<commit_message>
change the demand structure
</commit_message>
<xml_diff>
--- a/data/correlation/regression.xlsx
+++ b/data/correlation/regression.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoshinoriokubo/Documents/simulator/data/correlation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26231F01-1C4A-1244-839A-C088D3132FB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAD84F7-AEF2-054F-A77C-3599754BBABD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="460" windowWidth="27900" windowHeight="15400" xr2:uid="{CA90CC09-E6FD-5A43-8559-1E712E5E9A16}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27900" windowHeight="15400" xr2:uid="{CA90CC09-E6FD-5A43-8559-1E712E5E9A16}"/>
   </bookViews>
   <sheets>
     <sheet name="元データ" sheetId="1" r:id="rId1"/>
     <sheet name="往路運賃" sheetId="3" r:id="rId2"/>
     <sheet name="復路運賃" sheetId="4" r:id="rId3"/>
     <sheet name="新船価格" sheetId="6" r:id="rId4"/>
-    <sheet name="中古船価格" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId5"/>
+    <sheet name="中古船価格" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="37">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2"/>
@@ -648,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201083BE-F943-2C42-9F81-81E38B44A9E5}">
   <dimension ref="A1:K258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="J98" sqref="J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1067,7 +1068,7 @@
         <v>70.106220458766998</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:11">
       <c r="A49" s="1">
         <v>37956</v>
       </c>
@@ -1075,7 +1076,7 @@
         <v>72.070557732281259</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:11">
       <c r="A50" s="1">
         <v>37987</v>
       </c>
@@ -1085,8 +1086,12 @@
       <c r="I50">
         <v>72.4280742682447</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="K50">
+        <f>1000000*I50</f>
+        <v>72428074.268244699</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" s="1">
         <v>38018</v>
       </c>
@@ -1096,8 +1101,12 @@
       <c r="I51">
         <v>73.681852408114494</v>
       </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="K51">
+        <f t="shared" ref="K51:K114" si="0">1000000*I51</f>
+        <v>73681852.408114493</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" s="1">
         <v>38047</v>
       </c>
@@ -1107,8 +1116,12 @@
       <c r="I52">
         <v>78.070075897658896</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="K52">
+        <f t="shared" si="0"/>
+        <v>78070075.897658899</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53" s="1">
         <v>38078</v>
       </c>
@@ -1118,8 +1131,12 @@
       <c r="I53">
         <v>80.891076712366001</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="K53">
+        <f t="shared" si="0"/>
+        <v>80891076.712366</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" s="1">
         <v>38108</v>
       </c>
@@ -1129,8 +1146,12 @@
       <c r="I54">
         <v>82.144854852235795</v>
       </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="K54">
+        <f t="shared" si="0"/>
+        <v>82144854.852235794</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="1">
         <v>38139</v>
       </c>
@@ -1140,8 +1161,12 @@
       <c r="I55">
         <v>83.085188457138202</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="K55">
+        <f t="shared" si="0"/>
+        <v>83085188.457138196</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" s="1">
         <v>38169</v>
       </c>
@@ -1151,8 +1176,12 @@
       <c r="I56">
         <v>83.398632992105703</v>
       </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="K56">
+        <f t="shared" si="0"/>
+        <v>83398632.992105708</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="1">
         <v>38200</v>
       </c>
@@ -1162,8 +1191,12 @@
       <c r="I57">
         <v>83.712077527073205</v>
       </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="K57">
+        <f t="shared" si="0"/>
+        <v>83712077.527073205</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" s="1">
         <v>38231</v>
       </c>
@@ -1173,8 +1206,12 @@
       <c r="I58">
         <v>85.906189271845307</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="K58">
+        <f t="shared" si="0"/>
+        <v>85906189.271845311</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" s="1">
         <v>38261</v>
       </c>
@@ -1184,8 +1221,12 @@
       <c r="I59">
         <v>87.473411946682603</v>
       </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="K59">
+        <f t="shared" si="0"/>
+        <v>87473411.946682602</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" s="1">
         <v>38292</v>
       </c>
@@ -1195,8 +1236,12 @@
       <c r="I60">
         <v>88.413745551584995</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="K60">
+        <f t="shared" si="0"/>
+        <v>88413745.551584989</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" s="1">
         <v>38322</v>
       </c>
@@ -1216,8 +1261,12 @@
       <c r="I61">
         <v>89.980968226422306</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="K61">
+        <f t="shared" si="0"/>
+        <v>89980968.22642231</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62" s="1">
         <v>38353</v>
       </c>
@@ -1234,8 +1283,12 @@
       <c r="I62">
         <v>92.801969041129396</v>
       </c>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="K62">
+        <f t="shared" si="0"/>
+        <v>92801969.041129395</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63" s="1">
         <v>38384</v>
       </c>
@@ -1252,8 +1305,12 @@
       <c r="I63">
         <v>93.115413576096898</v>
       </c>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="K63">
+        <f t="shared" si="0"/>
+        <v>93115413.576096892</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64" s="1">
         <v>38412</v>
       </c>
@@ -1264,14 +1321,18 @@
         <v>7473.75</v>
       </c>
       <c r="E64">
-        <f t="shared" ref="E64:E125" si="0">B64/D64</f>
+        <f t="shared" ref="E64:E125" si="1">B64/D64</f>
         <v>1.0884281015195438E-2</v>
       </c>
       <c r="I64">
         <v>97.817081600608702</v>
       </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="K64">
+        <f t="shared" si="0"/>
+        <v>97817081.600608706</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" s="1">
         <v>38443</v>
       </c>
@@ -1282,14 +1343,18 @@
         <v>7552</v>
       </c>
       <c r="E65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0689973828084799E-2</v>
       </c>
       <c r="I65">
         <v>102.51874962511999</v>
       </c>
-    </row>
-    <row r="66" spans="1:9">
+      <c r="K65">
+        <f t="shared" si="0"/>
+        <v>102518749.62512</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" s="1">
         <v>38473</v>
       </c>
@@ -1300,14 +1365,18 @@
         <v>7630.25</v>
       </c>
       <c r="E66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.045894533466638E-2</v>
       </c>
       <c r="I66">
         <v>102.205305090153</v>
       </c>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="K66">
+        <f t="shared" si="0"/>
+        <v>102205305.09015301</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67" s="1">
         <v>38504</v>
       </c>
@@ -1318,14 +1387,18 @@
         <v>7708.5</v>
       </c>
       <c r="E67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0230631997502355E-2</v>
       </c>
       <c r="I67">
         <v>99.070859740478596</v>
       </c>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="K67">
+        <f t="shared" si="0"/>
+        <v>99070859.74047859</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68" s="1">
         <v>38534</v>
       </c>
@@ -1336,14 +1409,18 @@
         <v>7786.75</v>
       </c>
       <c r="E68">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0175863247111325E-2</v>
       </c>
       <c r="I68">
         <v>97.190192530673798</v>
       </c>
-    </row>
-    <row r="69" spans="1:9">
+      <c r="K68">
+        <f t="shared" si="0"/>
+        <v>97190192.530673802</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69" s="1">
         <v>38565</v>
       </c>
@@ -1354,14 +1431,18 @@
         <v>7865</v>
       </c>
       <c r="E69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0273315507781489E-2</v>
       </c>
       <c r="I69">
         <v>93.742302646031803</v>
       </c>
-    </row>
-    <row r="70" spans="1:9">
+      <c r="K69">
+        <f t="shared" si="0"/>
+        <v>93742302.646031797</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70" s="1">
         <v>38596</v>
       </c>
@@ -1372,14 +1453,18 @@
         <v>7943.25</v>
       </c>
       <c r="E70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0270708348544702E-2</v>
       </c>
       <c r="I70">
         <v>90.921301831324698</v>
       </c>
-    </row>
-    <row r="71" spans="1:9">
+      <c r="K70">
+        <f t="shared" si="0"/>
+        <v>90921301.831324697</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71" s="1">
         <v>38626</v>
       </c>
@@ -1390,14 +1475,18 @@
         <v>8021.5</v>
       </c>
       <c r="E71">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0077071210012417E-2</v>
       </c>
       <c r="I71">
         <v>90.294412761389694</v>
       </c>
-    </row>
-    <row r="72" spans="1:9">
+      <c r="K71">
+        <f t="shared" si="0"/>
+        <v>90294412.761389688</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72" s="1">
         <v>38657</v>
       </c>
@@ -1408,14 +1497,18 @@
         <v>8099.75</v>
       </c>
       <c r="E72">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.863152438915725E-3</v>
       </c>
       <c r="I72">
         <v>89.667523691454804</v>
       </c>
-    </row>
-    <row r="73" spans="1:9">
+      <c r="K72">
+        <f t="shared" si="0"/>
+        <v>89667523.691454798</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73" s="1">
         <v>38687</v>
       </c>
@@ -1429,14 +1522,18 @@
         <v>8178</v>
       </c>
       <c r="E73">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.8763896872616115E-3</v>
       </c>
       <c r="I73">
         <v>89.040634621519899</v>
       </c>
-    </row>
-    <row r="74" spans="1:9">
+      <c r="K73">
+        <f t="shared" si="0"/>
+        <v>89040634.621519893</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74" s="1">
         <v>38718</v>
       </c>
@@ -1447,7 +1544,7 @@
         <v>8289.75</v>
       </c>
       <c r="E74">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.9436701373374417E-3</v>
       </c>
       <c r="F74">
@@ -1456,8 +1553,12 @@
       <c r="I74">
         <v>89.667523691454804</v>
       </c>
-    </row>
-    <row r="75" spans="1:9">
+      <c r="K74">
+        <f t="shared" si="0"/>
+        <v>89667523.691454798</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
       <c r="A75" s="1">
         <v>38749</v>
       </c>
@@ -1468,7 +1569,7 @@
         <v>8401.5</v>
       </c>
       <c r="E75">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.7678561883794684E-3</v>
       </c>
       <c r="F75">
@@ -1477,8 +1578,12 @@
       <c r="I75">
         <v>90.921301831324698</v>
       </c>
-    </row>
-    <row r="76" spans="1:9">
+      <c r="K75">
+        <f t="shared" si="0"/>
+        <v>90921301.831324697</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76" s="1">
         <v>38777</v>
       </c>
@@ -1489,7 +1594,7 @@
         <v>8513.25</v>
       </c>
       <c r="E76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.6811163421107252E-3</v>
       </c>
       <c r="F76">
@@ -1498,8 +1603,12 @@
       <c r="I76">
         <v>93.115413576096898</v>
       </c>
-    </row>
-    <row r="77" spans="1:9">
+      <c r="K76">
+        <f t="shared" si="0"/>
+        <v>93115413.576096892</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77" s="1">
         <v>38808</v>
       </c>
@@ -1510,7 +1619,7 @@
         <v>8625</v>
       </c>
       <c r="E77">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.7107575557211119E-3</v>
       </c>
       <c r="F77">
@@ -1519,8 +1628,12 @@
       <c r="I77">
         <v>94.369191715966707</v>
       </c>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="K77">
+        <f t="shared" si="0"/>
+        <v>94369191.715966702</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" s="1">
         <v>38838</v>
       </c>
@@ -1531,7 +1644,7 @@
         <v>8736.75</v>
       </c>
       <c r="E78">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.884184928232901E-3</v>
       </c>
       <c r="F78">
@@ -1540,8 +1653,12 @@
       <c r="I78">
         <v>95.622969855836502</v>
       </c>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="K78">
+        <f t="shared" si="0"/>
+        <v>95622969.855836496</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79" s="1">
         <v>38869</v>
       </c>
@@ -1552,7 +1669,7 @@
         <v>8848.5</v>
       </c>
       <c r="E79">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.6474314288463852E-3</v>
       </c>
       <c r="F79">
@@ -1561,8 +1678,12 @@
       <c r="I79">
         <v>96.876747995706395</v>
       </c>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="K79">
+        <f t="shared" si="0"/>
+        <v>96876747.995706394</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
       <c r="A80" s="1">
         <v>38899</v>
       </c>
@@ -1573,7 +1694,7 @@
         <v>8960.25</v>
       </c>
       <c r="E80">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.6010803861814667E-3</v>
       </c>
       <c r="F80">
@@ -1582,8 +1703,12 @@
       <c r="I80">
         <v>98.443970670543607</v>
       </c>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="K80">
+        <f t="shared" si="0"/>
+        <v>98443970.670543611</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
       <c r="A81" s="1">
         <v>38930</v>
       </c>
@@ -1594,7 +1719,7 @@
         <v>9072</v>
       </c>
       <c r="E81">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.6047063336902553E-3</v>
       </c>
       <c r="F81">
@@ -1603,8 +1728,12 @@
       <c r="I81">
         <v>99.070859740478596</v>
       </c>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="K81">
+        <f t="shared" si="0"/>
+        <v>99070859.74047859</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
       <c r="A82" s="1">
         <v>38961</v>
       </c>
@@ -1615,7 +1744,7 @@
         <v>9183.75</v>
       </c>
       <c r="E82">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.4161017000395867E-3</v>
       </c>
       <c r="F82">
@@ -1624,8 +1753,12 @@
       <c r="I82">
         <v>99.384304275445999</v>
       </c>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="K82">
+        <f t="shared" si="0"/>
+        <v>99384304.275445998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
       <c r="A83" s="1">
         <v>38991</v>
       </c>
@@ -1636,7 +1769,7 @@
         <v>9295.5</v>
       </c>
       <c r="E83">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.1635406952533908E-3</v>
       </c>
       <c r="F83">
@@ -1645,8 +1778,12 @@
       <c r="I83">
         <v>100.638082415315</v>
       </c>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="K83">
+        <f t="shared" si="0"/>
+        <v>100638082.415315</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
       <c r="A84" s="1">
         <v>39022</v>
       </c>
@@ -1657,7 +1794,7 @@
         <v>9407.25</v>
       </c>
       <c r="E84">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.1618440596280375E-3</v>
       </c>
       <c r="F84">
@@ -1666,8 +1803,12 @@
       <c r="I84">
         <v>100.32463788034801</v>
       </c>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="K84">
+        <f t="shared" si="0"/>
+        <v>100324637.88034801</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
       <c r="A85" s="1">
         <v>39052</v>
       </c>
@@ -1681,7 +1822,7 @@
         <v>9519</v>
       </c>
       <c r="E85">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.2894722379981195E-3</v>
       </c>
       <c r="F85">
@@ -1690,8 +1831,12 @@
       <c r="I85">
         <v>100.638082415315</v>
       </c>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="K85">
+        <f t="shared" si="0"/>
+        <v>100638082.415315</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
       <c r="A86" s="1">
         <v>39083</v>
       </c>
@@ -1702,7 +1847,7 @@
         <v>9627.5</v>
       </c>
       <c r="E86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.0347987149873125E-3</v>
       </c>
       <c r="F86">
@@ -1711,8 +1856,12 @@
       <c r="I86">
         <v>100.638082415315</v>
       </c>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="K86">
+        <f t="shared" si="0"/>
+        <v>100638082.415315</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
       <c r="A87" s="1">
         <v>39114</v>
       </c>
@@ -1723,7 +1872,7 @@
         <v>9736</v>
       </c>
       <c r="E87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.0027004732407614E-3</v>
       </c>
       <c r="F87">
@@ -1732,8 +1881,12 @@
       <c r="I87">
         <v>100.638082415315</v>
       </c>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="K87">
+        <f t="shared" si="0"/>
+        <v>100638082.415315</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
       <c r="A88" s="1">
         <v>39142</v>
       </c>
@@ -1744,7 +1897,7 @@
         <v>9844.5</v>
       </c>
       <c r="E88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.0327287226626141E-3</v>
       </c>
       <c r="F88">
@@ -1753,8 +1906,12 @@
       <c r="I88">
         <v>101.891860555185</v>
       </c>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="K88">
+        <f t="shared" si="0"/>
+        <v>101891860.55518501</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
       <c r="A89" s="1">
         <v>39173</v>
       </c>
@@ -1765,7 +1922,7 @@
         <v>9953</v>
       </c>
       <c r="E89">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.0659197544151054E-3</v>
       </c>
       <c r="F89">
@@ -1774,8 +1931,12 @@
       <c r="I89">
         <v>102.83219416008799</v>
       </c>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="K89">
+        <f t="shared" si="0"/>
+        <v>102832194.16008799</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
       <c r="A90" s="1">
         <v>39203</v>
       </c>
@@ -1786,7 +1947,7 @@
         <v>10061.5</v>
       </c>
       <c r="E90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.0321781832385876E-3</v>
       </c>
       <c r="F90">
@@ -1795,8 +1956,12 @@
       <c r="I90">
         <v>104.39941683492501</v>
       </c>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="K90">
+        <f t="shared" si="0"/>
+        <v>104399416.83492501</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
       <c r="A91" s="1">
         <v>39234</v>
       </c>
@@ -1807,7 +1972,7 @@
         <v>10170</v>
       </c>
       <c r="E91">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.9504429210579932E-3</v>
       </c>
       <c r="F91">
@@ -1816,8 +1981,12 @@
       <c r="I91">
         <v>104.39941683492501</v>
       </c>
-    </row>
-    <row r="92" spans="1:9">
+      <c r="K91">
+        <f t="shared" si="0"/>
+        <v>104399416.83492501</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
       <c r="A92" s="1">
         <v>39264</v>
       </c>
@@ -1828,7 +1997,7 @@
         <v>10278.5</v>
       </c>
       <c r="E92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.0224507189547408E-3</v>
       </c>
       <c r="F92">
@@ -1837,8 +2006,12 @@
       <c r="I92">
         <v>105.02630590486</v>
       </c>
-    </row>
-    <row r="93" spans="1:9">
+      <c r="K92">
+        <f t="shared" si="0"/>
+        <v>105026305.90485999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
       <c r="A93" s="1">
         <v>39295</v>
       </c>
@@ -1849,7 +2022,7 @@
         <v>10387</v>
       </c>
       <c r="E93">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.89151709029962E-3</v>
       </c>
       <c r="F93">
@@ -1858,8 +2031,12 @@
       <c r="I93">
         <v>104.712861369892</v>
       </c>
-    </row>
-    <row r="94" spans="1:9">
+      <c r="K93">
+        <f t="shared" si="0"/>
+        <v>104712861.369892</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
       <c r="A94" s="1">
         <v>39326</v>
       </c>
@@ -1870,7 +2047,7 @@
         <v>10495.5</v>
       </c>
       <c r="E94">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.9898135395879378E-3</v>
       </c>
       <c r="F94">
@@ -1879,8 +2056,12 @@
       <c r="I94">
         <v>105.02630590486</v>
       </c>
-    </row>
-    <row r="95" spans="1:9">
+      <c r="K94">
+        <f t="shared" si="0"/>
+        <v>105026305.90485999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
       <c r="A95" s="1">
         <v>39356</v>
       </c>
@@ -1891,7 +2072,7 @@
         <v>10604</v>
       </c>
       <c r="E95">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.1234053650889515E-3</v>
       </c>
       <c r="F95">
@@ -1900,8 +2081,12 @@
       <c r="I95">
         <v>105.02630590486</v>
       </c>
-    </row>
-    <row r="96" spans="1:9">
+      <c r="K95">
+        <f t="shared" si="0"/>
+        <v>105026305.90485999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
       <c r="A96" s="1">
         <v>39387</v>
       </c>
@@ -1912,7 +2097,7 @@
         <v>10712.5</v>
       </c>
       <c r="E96">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.3037849354333721E-3</v>
       </c>
       <c r="F96">
@@ -1921,8 +2106,12 @@
       <c r="I96">
         <v>105.02630590486</v>
       </c>
-    </row>
-    <row r="97" spans="1:10">
+      <c r="K96">
+        <f t="shared" si="0"/>
+        <v>105026305.90485999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
       <c r="A97" s="1">
         <v>39417</v>
       </c>
@@ -1936,7 +2125,7 @@
         <v>10821</v>
       </c>
       <c r="E97">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.2328754100073299E-3</v>
       </c>
       <c r="F97">
@@ -1945,8 +2134,12 @@
       <c r="I97">
         <v>105.653194974795</v>
       </c>
-    </row>
-    <row r="98" spans="1:10">
+      <c r="K97">
+        <f t="shared" si="0"/>
+        <v>105653194.974795</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
       <c r="A98" s="1">
         <v>39448</v>
       </c>
@@ -1957,7 +2150,7 @@
         <v>10931</v>
       </c>
       <c r="E98">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.3197174143472249E-3</v>
       </c>
       <c r="F98">
@@ -1969,8 +2162,12 @@
       <c r="J98">
         <v>109.74746839095801</v>
       </c>
-    </row>
-    <row r="99" spans="1:10">
+      <c r="K98">
+        <f t="shared" si="0"/>
+        <v>105339750.439827</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
       <c r="A99" s="1">
         <v>39479</v>
       </c>
@@ -1981,7 +2178,7 @@
         <v>11041</v>
       </c>
       <c r="E99">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.3793260223560375E-3</v>
       </c>
       <c r="F99">
@@ -1993,8 +2190,12 @@
       <c r="J99">
         <v>110.26553572713399</v>
       </c>
-    </row>
-    <row r="100" spans="1:10">
+      <c r="K99">
+        <f t="shared" si="0"/>
+        <v>105653194.974795</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
       <c r="A100" s="1">
         <v>39508</v>
       </c>
@@ -2005,7 +2206,7 @@
         <v>11151</v>
       </c>
       <c r="E100">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.6483870760402657E-3</v>
       </c>
       <c r="F100">
@@ -2017,8 +2218,12 @@
       <c r="J100">
         <v>108.970367386695</v>
       </c>
-    </row>
-    <row r="101" spans="1:10">
+      <c r="K100">
+        <f t="shared" si="0"/>
+        <v>105653194.974795</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
       <c r="A101" s="1">
         <v>39539</v>
       </c>
@@ -2029,7 +2234,7 @@
         <v>11261</v>
       </c>
       <c r="E101">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.6929700412120151E-3</v>
       </c>
       <c r="F101">
@@ -2041,8 +2246,12 @@
       <c r="J101">
         <v>108.970367386695</v>
       </c>
-    </row>
-    <row r="102" spans="1:10">
+      <c r="K101">
+        <f t="shared" si="0"/>
+        <v>105966639.509762</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
       <c r="A102" s="1">
         <v>39569</v>
       </c>
@@ -2053,7 +2262,7 @@
         <v>11371</v>
       </c>
       <c r="E102">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.6693881834347458E-3</v>
       </c>
       <c r="F102">
@@ -2065,8 +2274,12 @@
       <c r="J102">
         <v>107.15713171007999</v>
       </c>
-    </row>
-    <row r="103" spans="1:10">
+      <c r="K102">
+        <f t="shared" si="0"/>
+        <v>105966639.509762</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
       <c r="A103" s="1">
         <v>39600</v>
       </c>
@@ -2077,7 +2290,7 @@
         <v>11481</v>
       </c>
       <c r="E103">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.743110200694757E-3</v>
       </c>
       <c r="F103">
@@ -2089,8 +2302,12 @@
       <c r="J103">
         <v>101.97645834832301</v>
       </c>
-    </row>
-    <row r="104" spans="1:10">
+      <c r="K103">
+        <f t="shared" si="0"/>
+        <v>105966639.509762</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
       <c r="A104" s="1">
         <v>39630</v>
       </c>
@@ -2101,7 +2318,7 @@
         <v>11591</v>
       </c>
       <c r="E104">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.8461799313284432E-3</v>
       </c>
       <c r="F104">
@@ -2113,8 +2330,12 @@
       <c r="J104">
         <v>102.494525684499</v>
       </c>
-    </row>
-    <row r="105" spans="1:10">
+      <c r="K104">
+        <f t="shared" si="0"/>
+        <v>106280084.04473001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
       <c r="A105" s="1">
         <v>39661</v>
       </c>
@@ -2125,7 +2346,7 @@
         <v>11701</v>
       </c>
       <c r="E105">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.4417845502810863E-3</v>
       </c>
       <c r="F105">
@@ -2137,8 +2358,12 @@
       <c r="J105">
         <v>103.53066035685001</v>
       </c>
-    </row>
-    <row r="106" spans="1:10">
+      <c r="K105">
+        <f t="shared" si="0"/>
+        <v>106280084.04473001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
       <c r="A106" s="1">
         <v>39692</v>
       </c>
@@ -2149,7 +2374,7 @@
         <v>11811</v>
       </c>
       <c r="E106">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.0399276152029473E-3</v>
       </c>
       <c r="F106">
@@ -2161,8 +2386,12 @@
       <c r="J106">
         <v>98.090953327005707</v>
       </c>
-    </row>
-    <row r="107" spans="1:10">
+      <c r="K106">
+        <f t="shared" si="0"/>
+        <v>105653194.974795</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
       <c r="A107" s="1">
         <v>39722</v>
       </c>
@@ -2173,7 +2402,7 @@
         <v>11921</v>
       </c>
       <c r="E107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.3838439293373417E-3</v>
       </c>
       <c r="F107">
@@ -2185,8 +2414,12 @@
       <c r="J107">
         <v>86.434438263052797</v>
       </c>
-    </row>
-    <row r="108" spans="1:10">
+      <c r="K107">
+        <f t="shared" si="0"/>
+        <v>103459083.230023</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
       <c r="A108" s="1">
         <v>39753</v>
       </c>
@@ -2197,7 +2430,7 @@
         <v>12031</v>
       </c>
       <c r="E108">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.8292238287929437E-3</v>
       </c>
       <c r="F108">
@@ -2209,8 +2442,12 @@
       <c r="J108">
         <v>74.518889531012107</v>
       </c>
-    </row>
-    <row r="109" spans="1:10">
+      <c r="K108">
+        <f t="shared" si="0"/>
+        <v>99697748.810413495</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
       <c r="A109" s="1">
         <v>39783</v>
       </c>
@@ -2224,7 +2461,7 @@
         <v>12141</v>
       </c>
       <c r="E109">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.7037940116687666E-3</v>
       </c>
       <c r="F109">
@@ -2236,8 +2473,12 @@
       <c r="J109">
         <v>70.115317173518804</v>
       </c>
-    </row>
-    <row r="110" spans="1:10">
+      <c r="K109">
+        <f t="shared" si="0"/>
+        <v>97190192.530673802</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
       <c r="A110" s="1">
         <v>39814</v>
       </c>
@@ -2248,7 +2489,7 @@
         <v>12207.416666666666</v>
       </c>
       <c r="E110">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4365574041813749E-3</v>
       </c>
       <c r="F110">
@@ -2260,8 +2501,12 @@
       <c r="J110">
         <v>68.302081496903895</v>
       </c>
-    </row>
-    <row r="111" spans="1:10">
+      <c r="K110">
+        <f t="shared" si="0"/>
+        <v>94682636.250934094</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11">
       <c r="A111" s="1">
         <v>39845</v>
       </c>
@@ -2272,7 +2517,7 @@
         <v>12273.833333333334</v>
       </c>
       <c r="E111">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.2176710500924035E-3</v>
       </c>
       <c r="F111">
@@ -2284,8 +2529,12 @@
       <c r="J111">
         <v>66.488845820289001</v>
       </c>
-    </row>
-    <row r="112" spans="1:10">
+      <c r="K111">
+        <f t="shared" si="0"/>
+        <v>89040634.621519893</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11">
       <c r="A112" s="1">
         <v>39873</v>
       </c>
@@ -2296,7 +2545,7 @@
         <v>12340.25</v>
       </c>
       <c r="E112">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.1942682451715274E-3</v>
       </c>
       <c r="F112">
@@ -2308,8 +2557,12 @@
       <c r="J112">
         <v>64.675610143674206</v>
       </c>
-    </row>
-    <row r="113" spans="1:10">
+      <c r="K112">
+        <f t="shared" si="0"/>
+        <v>86533078.34178029</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
       <c r="A113" s="1">
         <v>39904</v>
       </c>
@@ -2320,7 +2573,7 @@
         <v>12406.666666666666</v>
       </c>
       <c r="E113">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.1400561914398142E-3</v>
       </c>
       <c r="F113">
@@ -2332,8 +2585,12 @@
       <c r="J113">
         <v>63.121408135147099</v>
       </c>
-    </row>
-    <row r="114" spans="1:10">
+      <c r="K113">
+        <f t="shared" si="0"/>
+        <v>83712077.5270731</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11">
       <c r="A114" s="1">
         <v>39934</v>
       </c>
@@ -2344,7 +2601,7 @@
         <v>12473.083333333334</v>
       </c>
       <c r="E114">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.2782011705324733E-3</v>
       </c>
       <c r="F114">
@@ -2356,8 +2613,12 @@
       <c r="J114">
         <v>59.753970450005198</v>
       </c>
-    </row>
-    <row r="115" spans="1:10">
+      <c r="K114">
+        <f t="shared" si="0"/>
+        <v>80264187.642431095</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11">
       <c r="A115" s="1">
         <v>39965</v>
       </c>
@@ -2368,7 +2629,7 @@
         <v>12539.5</v>
       </c>
       <c r="E115">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4301200931874241E-3</v>
       </c>
       <c r="F115">
@@ -2380,8 +2641,12 @@
       <c r="J115">
         <v>53.278128747809099</v>
       </c>
-    </row>
-    <row r="116" spans="1:10">
+      <c r="K115">
+        <f t="shared" ref="K115:K178" si="2">1000000*I115</f>
+        <v>76502853.222821593</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11">
       <c r="A116" s="1">
         <v>39995</v>
       </c>
@@ -2392,7 +2657,7 @@
         <v>12605.916666666666</v>
       </c>
       <c r="E116">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4283004453661126E-3</v>
       </c>
       <c r="F116">
@@ -2404,8 +2669,12 @@
       <c r="J116">
         <v>48.356489054140098</v>
       </c>
-    </row>
-    <row r="117" spans="1:10">
+      <c r="K116">
+        <f t="shared" si="2"/>
+        <v>75249075.082951799</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
       <c r="A117" s="1">
         <v>40026</v>
       </c>
@@ -2416,7 +2685,7 @@
         <v>12672.333333333334</v>
       </c>
       <c r="E117">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.511472509997565E-3</v>
       </c>
       <c r="F117">
@@ -2428,8 +2697,12 @@
       <c r="J117">
         <v>47.061320713700901</v>
       </c>
-    </row>
-    <row r="118" spans="1:10">
+      <c r="K117">
+        <f t="shared" si="2"/>
+        <v>72114629.733277202</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11">
       <c r="A118" s="1">
         <v>40057</v>
       </c>
@@ -2440,7 +2713,7 @@
         <v>12738.75</v>
       </c>
       <c r="E118">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.5728730709438532E-3</v>
       </c>
       <c r="F118">
@@ -2452,8 +2725,12 @@
       <c r="J118">
         <v>46.543253377525197</v>
       </c>
-    </row>
-    <row r="119" spans="1:10">
+      <c r="K118">
+        <f t="shared" si="2"/>
+        <v>70233962.523472399</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11">
       <c r="A119" s="1">
         <v>40087</v>
       </c>
@@ -2464,7 +2741,7 @@
         <v>12805.166666666666</v>
       </c>
       <c r="E119">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.6453126984677051E-3</v>
       </c>
       <c r="F119">
@@ -2476,8 +2753,12 @@
       <c r="J119">
         <v>43.952916696646803</v>
       </c>
-    </row>
-    <row r="120" spans="1:10">
+      <c r="K119">
+        <f t="shared" si="2"/>
+        <v>67726406.243732795</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11">
       <c r="A120" s="1">
         <v>40118</v>
       </c>
@@ -2488,7 +2769,7 @@
         <v>12871.583333333334</v>
       </c>
       <c r="E120">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.6927682498140262E-3</v>
       </c>
       <c r="F120">
@@ -2500,8 +2781,12 @@
       <c r="J120">
         <v>42.657748356207598</v>
       </c>
-    </row>
-    <row r="121" spans="1:10">
+      <c r="K120">
+        <f t="shared" si="2"/>
+        <v>67726406.243732795</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11">
       <c r="A121" s="1">
         <v>40148</v>
       </c>
@@ -2515,7 +2800,7 @@
         <v>12938</v>
       </c>
       <c r="E121">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.6304868906664205E-3</v>
       </c>
       <c r="F121">
@@ -2527,8 +2812,12 @@
       <c r="J121">
         <v>41.103546347680499</v>
       </c>
-    </row>
-    <row r="122" spans="1:10">
+      <c r="K121">
+        <f t="shared" si="2"/>
+        <v>67412961.708765298</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
       <c r="A122" s="1">
         <v>40179</v>
       </c>
@@ -2539,7 +2828,7 @@
         <v>13034.166666666666</v>
       </c>
       <c r="E122">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.6160329449575332E-3</v>
       </c>
       <c r="F122">
@@ -2551,8 +2840,12 @@
       <c r="J122">
         <v>43.434849360471098</v>
       </c>
-    </row>
-    <row r="123" spans="1:10">
+      <c r="K122">
+        <f t="shared" si="2"/>
+        <v>66786072.638830401</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
       <c r="A123" s="1">
         <v>40210</v>
       </c>
@@ -2563,7 +2856,7 @@
         <v>13130.333333333334</v>
       </c>
       <c r="E123">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4298267882140249E-3</v>
       </c>
       <c r="F123">
@@ -2575,8 +2868,12 @@
       <c r="J123">
         <v>46.543253377525197</v>
       </c>
-    </row>
-    <row r="124" spans="1:10">
+      <c r="K123">
+        <f t="shared" si="2"/>
+        <v>66786072.638830401</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
       <c r="A124" s="1">
         <v>40238</v>
       </c>
@@ -2587,7 +2884,7 @@
         <v>13226.5</v>
       </c>
       <c r="E124">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4466880252908674E-3</v>
       </c>
       <c r="F124">
@@ -2599,8 +2896,12 @@
       <c r="J124">
         <v>50.687792066930697</v>
       </c>
-    </row>
-    <row r="125" spans="1:10">
+      <c r="K124">
+        <f t="shared" si="2"/>
+        <v>67099517.173797905</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
       <c r="A125" s="1">
         <v>40269</v>
       </c>
@@ -2611,7 +2912,7 @@
         <v>13322.666666666666</v>
       </c>
       <c r="E125">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4357656453540345E-3</v>
       </c>
       <c r="F125">
@@ -2623,8 +2924,12 @@
       <c r="J125">
         <v>52.760061411633401</v>
       </c>
-    </row>
-    <row r="126" spans="1:10">
+      <c r="K125">
+        <f t="shared" si="2"/>
+        <v>67412961.708765298</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
       <c r="A126" s="1">
         <v>40299</v>
       </c>
@@ -2635,7 +2940,7 @@
         <v>13418.833333333334</v>
       </c>
       <c r="E126">
-        <f t="shared" ref="E126:E189" si="1">B126/D126</f>
+        <f t="shared" ref="E126:E189" si="3">B126/D126</f>
         <v>7.2211473071971087E-3</v>
       </c>
       <c r="F126">
@@ -2647,8 +2952,12 @@
       <c r="J126">
         <v>55.8684654286875</v>
       </c>
-    </row>
-    <row r="127" spans="1:10">
+      <c r="K126">
+        <f t="shared" si="2"/>
+        <v>66786072.638830401</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11">
       <c r="A127" s="1">
         <v>40330</v>
       </c>
@@ -2659,7 +2968,7 @@
         <v>13515</v>
       </c>
       <c r="E127">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.1348114149456165E-3</v>
       </c>
       <c r="F127">
@@ -2671,8 +2980,12 @@
       <c r="J127">
         <v>57.681701105302402</v>
       </c>
-    </row>
-    <row r="128" spans="1:10">
+      <c r="K127">
+        <f t="shared" si="2"/>
+        <v>67726406.243732795</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
       <c r="A128" s="1">
         <v>40360</v>
       </c>
@@ -2683,7 +2996,7 @@
         <v>13611.166666666666</v>
       </c>
       <c r="E128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.2491453429729168E-3</v>
       </c>
       <c r="F128">
@@ -2695,8 +3008,12 @@
       <c r="J128">
         <v>59.753970450005099</v>
       </c>
-    </row>
-    <row r="129" spans="1:10">
+      <c r="K128">
+        <f t="shared" si="2"/>
+        <v>71174296.1283748</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11">
       <c r="A129" s="1">
         <v>40391</v>
       </c>
@@ -2707,7 +3024,7 @@
         <v>13707.333333333334</v>
       </c>
       <c r="E129">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.2744414049674055E-3</v>
       </c>
       <c r="F129">
@@ -2719,8 +3036,12 @@
       <c r="J129">
         <v>65.970778484113296</v>
       </c>
-    </row>
-    <row r="130" spans="1:10">
+      <c r="K129">
+        <f t="shared" si="2"/>
+        <v>74935630.547984302</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11">
       <c r="A130" s="1">
         <v>40422</v>
       </c>
@@ -2731,7 +3052,7 @@
         <v>13803.5</v>
       </c>
       <c r="E130">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.2961154517752732E-3</v>
       </c>
       <c r="F130">
@@ -2743,8 +3064,12 @@
       <c r="J130">
         <v>67.784014160728205</v>
       </c>
-    </row>
-    <row r="131" spans="1:10">
+      <c r="K130">
+        <f t="shared" si="2"/>
+        <v>76189408.687854096</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11">
       <c r="A131" s="1">
         <v>40452</v>
       </c>
@@ -2755,7 +3080,7 @@
         <v>13899.666666666666</v>
       </c>
       <c r="E131">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.4928985520909498E-3</v>
       </c>
       <c r="F131">
@@ -2767,8 +3092,12 @@
       <c r="J131">
         <v>68.8201488330796</v>
       </c>
-    </row>
-    <row r="132" spans="1:10">
+      <c r="K131">
+        <f t="shared" si="2"/>
+        <v>77129742.292756498</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11">
       <c r="A132" s="1">
         <v>40483</v>
       </c>
@@ -2779,7 +3108,7 @@
         <v>13995.833333333334</v>
       </c>
       <c r="E132">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.4614404656274964E-3</v>
       </c>
       <c r="F132">
@@ -2791,8 +3120,12 @@
       <c r="J132">
         <v>70.115317173518804</v>
       </c>
-    </row>
-    <row r="133" spans="1:10">
+      <c r="K132">
+        <f t="shared" si="2"/>
+        <v>78070075.897658899</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11">
       <c r="A133" s="1">
         <v>40513</v>
       </c>
@@ -2806,7 +3139,7 @@
         <v>14092</v>
       </c>
       <c r="E133">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.4239811605591828E-3</v>
       </c>
       <c r="F133">
@@ -2818,8 +3151,12 @@
       <c r="J133">
         <v>71.410485513957994</v>
       </c>
-    </row>
-    <row r="134" spans="1:10">
+      <c r="K133">
+        <f t="shared" si="2"/>
+        <v>77443186.82772401</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11">
       <c r="A134" s="1">
         <v>40544</v>
       </c>
@@ -2830,7 +3167,7 @@
         <v>14194.25</v>
       </c>
       <c r="E134">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.5930144855099781E-3</v>
       </c>
       <c r="F134">
@@ -2848,8 +3185,12 @@
       <c r="J134">
         <v>71.928552850133698</v>
       </c>
-    </row>
-    <row r="135" spans="1:10">
+      <c r="K134">
+        <f t="shared" si="2"/>
+        <v>75249075.082951799</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11">
       <c r="A135" s="1">
         <v>40575</v>
       </c>
@@ -2860,7 +3201,7 @@
         <v>14296.5</v>
       </c>
       <c r="E135">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.6918273901582903E-3</v>
       </c>
       <c r="F135">
@@ -2878,8 +3219,12 @@
       <c r="J135">
         <v>72.964687522485093</v>
       </c>
-    </row>
-    <row r="136" spans="1:10">
+      <c r="K135">
+        <f t="shared" si="2"/>
+        <v>72428074.268244699</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11">
       <c r="A136" s="1">
         <v>40603</v>
       </c>
@@ -2890,7 +3235,7 @@
         <v>14398.75</v>
       </c>
       <c r="E136">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.8265236059516623E-3</v>
       </c>
       <c r="F136">
@@ -2908,8 +3253,12 @@
       <c r="J136">
         <v>74.259855862924297</v>
       </c>
-    </row>
-    <row r="137" spans="1:10">
+      <c r="K136">
+        <f t="shared" si="2"/>
+        <v>70860851.593407407</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11">
       <c r="A137" s="1">
         <v>40634</v>
       </c>
@@ -2920,7 +3269,7 @@
         <v>14501</v>
       </c>
       <c r="E137">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.9787382891049578E-3</v>
       </c>
       <c r="F137">
@@ -2938,8 +3287,12 @@
       <c r="J137">
         <v>74.777923199100002</v>
       </c>
-    </row>
-    <row r="138" spans="1:10">
+      <c r="K137">
+        <f t="shared" si="2"/>
+        <v>70547407.058439896</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11">
       <c r="A138" s="1">
         <v>40664</v>
       </c>
@@ -2950,7 +3303,7 @@
         <v>14603.25</v>
       </c>
       <c r="E138">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.908160595794942E-3</v>
       </c>
       <c r="F138">
@@ -2968,8 +3321,12 @@
       <c r="J138">
         <v>74.777923199100002</v>
       </c>
-    </row>
-    <row r="139" spans="1:10">
+      <c r="K138">
+        <f t="shared" si="2"/>
+        <v>70233962.523472399</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11">
       <c r="A139" s="1">
         <v>40695</v>
       </c>
@@ -2980,7 +3337,7 @@
         <v>14705.5</v>
       </c>
       <c r="E139">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.8764906887171127E-3</v>
       </c>
       <c r="F139">
@@ -2998,8 +3355,12 @@
       <c r="J139">
         <v>74.518889531012107</v>
       </c>
-    </row>
-    <row r="140" spans="1:10">
+      <c r="K139">
+        <f t="shared" si="2"/>
+        <v>70547407.058439896</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11">
       <c r="A140" s="1">
         <v>40725</v>
       </c>
@@ -3010,7 +3371,7 @@
         <v>14807.75</v>
       </c>
       <c r="E140">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.8588470329770902E-3</v>
       </c>
       <c r="F140">
@@ -3028,8 +3389,12 @@
       <c r="J140">
         <v>73.223721190572903</v>
       </c>
-    </row>
-    <row r="141" spans="1:10">
+      <c r="K140">
+        <f t="shared" si="2"/>
+        <v>69607073.453537494</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11">
       <c r="A141" s="1">
         <v>40756</v>
       </c>
@@ -3040,7 +3405,7 @@
         <v>14910</v>
       </c>
       <c r="E141">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.8417168977238435E-3</v>
       </c>
       <c r="F141">
@@ -3058,8 +3423,12 @@
       <c r="J141">
         <v>70.892418177782403</v>
       </c>
-    </row>
-    <row r="142" spans="1:10">
+      <c r="K141">
+        <f t="shared" si="2"/>
+        <v>69920517.988504991</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11">
       <c r="A142" s="1">
         <v>40787</v>
       </c>
@@ -3070,7 +3439,7 @@
         <v>15012.25</v>
       </c>
       <c r="E142">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.6188840874884178E-3</v>
       </c>
       <c r="F142">
@@ -3088,8 +3457,12 @@
       <c r="J142">
         <v>67.265946824552501</v>
       </c>
-    </row>
-    <row r="143" spans="1:10">
+      <c r="K142">
+        <f t="shared" si="2"/>
+        <v>69607073.453537598</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11">
       <c r="A143" s="1">
         <v>40817</v>
       </c>
@@ -3100,7 +3473,7 @@
         <v>15114.5</v>
       </c>
       <c r="E143">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.5724115167544745E-3</v>
       </c>
       <c r="F143">
@@ -3118,8 +3491,12 @@
       <c r="J143">
         <v>58.458802109565902</v>
       </c>
-    </row>
-    <row r="144" spans="1:10">
+      <c r="K143">
+        <f t="shared" si="2"/>
+        <v>68666739.848635107</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11">
       <c r="A144" s="1">
         <v>40848</v>
       </c>
@@ -3130,7 +3507,7 @@
         <v>15216.75</v>
       </c>
       <c r="E144">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.4910033329346282E-3</v>
       </c>
       <c r="F144">
@@ -3148,8 +3525,12 @@
       <c r="J144">
         <v>53.537162415896901</v>
       </c>
-    </row>
-    <row r="145" spans="1:10">
+      <c r="K144">
+        <f t="shared" si="2"/>
+        <v>68039850.778700203</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11">
       <c r="A145" s="1">
         <v>40878</v>
       </c>
@@ -3163,7 +3544,7 @@
         <v>15319</v>
       </c>
       <c r="E145">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.3642016660257856E-3</v>
       </c>
       <c r="F145">
@@ -3181,8 +3562,12 @@
       <c r="J145">
         <v>49.651657394579303</v>
       </c>
-    </row>
-    <row r="146" spans="1:10">
+      <c r="K145">
+        <f t="shared" si="2"/>
+        <v>67412961.708765298</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11">
       <c r="A146" s="1">
         <v>40909</v>
       </c>
@@ -3193,7 +3578,7 @@
         <v>15392.083333333334</v>
       </c>
       <c r="E146">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.3520317685656809E-3</v>
       </c>
       <c r="F146">
@@ -3211,8 +3596,12 @@
       <c r="J146">
         <v>49.651657394579303</v>
       </c>
-    </row>
-    <row r="147" spans="1:10">
+      <c r="K146">
+        <f t="shared" si="2"/>
+        <v>67099517.173797809</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11">
       <c r="A147" s="1">
         <v>40940</v>
       </c>
@@ -3223,7 +3612,7 @@
         <v>15465.166666666666</v>
       </c>
       <c r="E147">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.4370116398247031E-3</v>
       </c>
       <c r="F147">
@@ -3241,8 +3630,12 @@
       <c r="J147">
         <v>49.651657394579303</v>
       </c>
-    </row>
-    <row r="148" spans="1:10">
+      <c r="K147">
+        <f t="shared" si="2"/>
+        <v>66472628.103862904</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11">
       <c r="A148" s="1">
         <v>40969</v>
       </c>
@@ -3253,7 +3646,7 @@
         <v>15538.25</v>
       </c>
       <c r="E148">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.3862809020150601E-3</v>
       </c>
       <c r="F148">
@@ -3271,8 +3664,12 @@
       <c r="J148">
         <v>49.910691062667198</v>
       </c>
-    </row>
-    <row r="149" spans="1:10">
+      <c r="K148">
+        <f t="shared" si="2"/>
+        <v>65218849.963993095</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11">
       <c r="A149" s="1">
         <v>41000</v>
       </c>
@@ -3283,7 +3680,7 @@
         <v>15611.333333333334</v>
       </c>
       <c r="E149">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.3365940188571122E-3</v>
       </c>
       <c r="F149">
@@ -3301,8 +3698,12 @@
       <c r="J149">
         <v>50.169724730755</v>
       </c>
-    </row>
-    <row r="150" spans="1:10">
+      <c r="K149">
+        <f t="shared" si="2"/>
+        <v>63965071.824123301</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11">
       <c r="A150" s="1">
         <v>41030</v>
       </c>
@@ -3313,7 +3714,7 @@
         <v>15684.416666666666</v>
       </c>
       <c r="E150">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.1706798473676519E-3</v>
       </c>
       <c r="F150">
@@ -3331,8 +3732,12 @@
       <c r="J150">
         <v>50.9468257350185</v>
       </c>
-    </row>
-    <row r="151" spans="1:10">
+      <c r="K150">
+        <f t="shared" si="2"/>
+        <v>62711293.684253402</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11">
       <c r="A151" s="1">
         <v>41061</v>
       </c>
@@ -3343,7 +3748,7 @@
         <v>15757.5</v>
       </c>
       <c r="E151">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.0117125996866257E-3</v>
       </c>
       <c r="F151">
@@ -3361,8 +3766,12 @@
       <c r="J151">
         <v>50.9468257350185</v>
       </c>
-    </row>
-    <row r="152" spans="1:10">
+      <c r="K151">
+        <f t="shared" si="2"/>
+        <v>61457515.5443836</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11">
       <c r="A152" s="1">
         <v>41091</v>
       </c>
@@ -3373,7 +3782,7 @@
         <v>15830.583333333334</v>
       </c>
       <c r="E152">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.9316151463152753E-3</v>
       </c>
       <c r="F152">
@@ -3391,8 +3800,12 @@
       <c r="J152">
         <v>50.9468257350185</v>
       </c>
-    </row>
-    <row r="153" spans="1:10">
+      <c r="K152">
+        <f t="shared" si="2"/>
+        <v>60203737.404513799</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11">
       <c r="A153" s="1">
         <v>41122</v>
       </c>
@@ -3403,7 +3816,7 @@
         <v>15903.666666666666</v>
       </c>
       <c r="E153">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.977325379228648E-3</v>
       </c>
       <c r="F153">
@@ -3421,8 +3834,12 @@
       <c r="J153">
         <v>50.687792066930697</v>
       </c>
-    </row>
-    <row r="154" spans="1:10">
+      <c r="K153">
+        <f t="shared" si="2"/>
+        <v>59576848.334578902</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11">
       <c r="A154" s="1">
         <v>41153</v>
       </c>
@@ -3433,7 +3850,7 @@
         <v>15976.75</v>
       </c>
       <c r="E154">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.0760269946738225E-3</v>
       </c>
       <c r="F154">
@@ -3451,8 +3868,12 @@
       <c r="J154">
         <v>49.392623726491401</v>
       </c>
-    </row>
-    <row r="155" spans="1:10">
+      <c r="K154">
+        <f t="shared" si="2"/>
+        <v>59263403.799611405</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11">
       <c r="A155" s="1">
         <v>41183</v>
       </c>
@@ -3463,7 +3884,7 @@
         <v>16049.833333333334</v>
       </c>
       <c r="E155">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.0314645144978136E-3</v>
       </c>
       <c r="F155">
@@ -3481,8 +3902,12 @@
       <c r="J155">
         <v>48.356489054140098</v>
       </c>
-    </row>
-    <row r="156" spans="1:10">
+      <c r="K155">
+        <f t="shared" si="2"/>
+        <v>58949959.264644004</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11">
       <c r="A156" s="1">
         <v>41214</v>
       </c>
@@ -3493,7 +3918,7 @@
         <v>16122.916666666666</v>
       </c>
       <c r="E156">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.936367020158595E-3</v>
       </c>
       <c r="F156">
@@ -3511,8 +3936,12 @@
       <c r="J156">
         <v>47.061320713700901</v>
       </c>
-    </row>
-    <row r="157" spans="1:10">
+      <c r="K156">
+        <f t="shared" si="2"/>
+        <v>58009625.659741603</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11">
       <c r="A157" s="1">
         <v>41244</v>
       </c>
@@ -3526,7 +3955,7 @@
         <v>16196</v>
       </c>
       <c r="E157">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.9928032744378862E-3</v>
       </c>
       <c r="F157">
@@ -3544,8 +3973,12 @@
       <c r="J157">
         <v>46.543253377525197</v>
       </c>
-    </row>
-    <row r="158" spans="1:10">
+      <c r="K157">
+        <f t="shared" si="2"/>
+        <v>57382736.589806698</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11">
       <c r="A158" s="1">
         <v>41275</v>
       </c>
@@ -3556,7 +3989,7 @@
         <v>16274.25</v>
       </c>
       <c r="E158">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.9750081950806951E-3</v>
       </c>
       <c r="F158">
@@ -3574,8 +4007,12 @@
       <c r="J158">
         <v>47.838421717964401</v>
       </c>
-    </row>
-    <row r="159" spans="1:10">
+      <c r="K158">
+        <f t="shared" si="2"/>
+        <v>57069292.054839201</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11">
       <c r="A159" s="1">
         <v>41306</v>
       </c>
@@ -3586,7 +4023,7 @@
         <v>16352.5</v>
       </c>
       <c r="E159">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.9713501512195389E-3</v>
       </c>
       <c r="F159">
@@ -3604,8 +4041,12 @@
       <c r="J159">
         <v>49.910691062667198</v>
       </c>
-    </row>
-    <row r="160" spans="1:10">
+      <c r="K159">
+        <f t="shared" si="2"/>
+        <v>57382736.589806601</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11">
       <c r="A160" s="1">
         <v>41334</v>
       </c>
@@ -3616,7 +4057,7 @@
         <v>16430.75</v>
       </c>
       <c r="E160">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.853116418442615E-3</v>
       </c>
       <c r="F160">
@@ -3634,8 +4075,12 @@
       <c r="J160">
         <v>50.9468257350185</v>
       </c>
-    </row>
-    <row r="161" spans="1:10">
+      <c r="K160">
+        <f t="shared" si="2"/>
+        <v>57382736.589806698</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11">
       <c r="A161" s="1">
         <v>41365</v>
       </c>
@@ -3646,7 +4091,7 @@
         <v>16509</v>
       </c>
       <c r="E161">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.7851988566164515E-3</v>
       </c>
       <c r="F161">
@@ -3664,8 +4109,12 @@
       <c r="J161">
         <v>48.615522722227901</v>
       </c>
-    </row>
-    <row r="162" spans="1:10">
+      <c r="K161">
+        <f t="shared" si="2"/>
+        <v>58323070.194708996</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11">
       <c r="A162" s="1">
         <v>41395</v>
       </c>
@@ -3676,7 +4125,7 @@
         <v>16587.25</v>
       </c>
       <c r="E162">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.676943364553347E-3</v>
       </c>
       <c r="F162">
@@ -3694,8 +4143,12 @@
       <c r="J162">
         <v>48.615522722228</v>
       </c>
-    </row>
-    <row r="163" spans="1:10">
+      <c r="K162">
+        <f t="shared" si="2"/>
+        <v>58949959.264644004</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11">
       <c r="A163" s="1">
         <v>41426</v>
       </c>
@@ -3706,7 +4159,7 @@
         <v>16665.5</v>
       </c>
       <c r="E163">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.703183310315863E-3</v>
       </c>
       <c r="F163">
@@ -3724,8 +4177,12 @@
       <c r="J163">
         <v>49.651657394579303</v>
       </c>
-    </row>
-    <row r="164" spans="1:10">
+      <c r="K163">
+        <f t="shared" si="2"/>
+        <v>59263403.799611405</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11">
       <c r="A164" s="1">
         <v>41456</v>
       </c>
@@ -3736,7 +4193,7 @@
         <v>16743.75</v>
       </c>
       <c r="E164">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.6161343709795293E-3</v>
       </c>
       <c r="F164">
@@ -3754,8 +4211,12 @@
       <c r="J164">
         <v>50.9468257350185</v>
       </c>
-    </row>
-    <row r="165" spans="1:10">
+      <c r="K164">
+        <f t="shared" si="2"/>
+        <v>61457515.5443836</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11">
       <c r="A165" s="1">
         <v>41487</v>
       </c>
@@ -3766,7 +4227,7 @@
         <v>16822</v>
       </c>
       <c r="E165">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.6308533135467848E-3</v>
       </c>
       <c r="F165">
@@ -3784,8 +4245,12 @@
       <c r="J165">
         <v>51.205859403106402</v>
       </c>
-    </row>
-    <row r="166" spans="1:10">
+      <c r="K165">
+        <f t="shared" si="2"/>
+        <v>62397849.149286002</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11">
       <c r="A166" s="1">
         <v>41518</v>
       </c>
@@ -3796,7 +4261,7 @@
         <v>16900.25</v>
       </c>
       <c r="E166">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.6220454437312766E-3</v>
       </c>
       <c r="F166">
@@ -3814,8 +4279,12 @@
       <c r="J166">
         <v>51.464893071194197</v>
       </c>
-    </row>
-    <row r="167" spans="1:10">
+      <c r="K166">
+        <f t="shared" si="2"/>
+        <v>63651627.289155796</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11">
       <c r="A167" s="1">
         <v>41548</v>
       </c>
@@ -3826,7 +4295,7 @@
         <v>16978.5</v>
       </c>
       <c r="E167">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.6206356169350644E-3</v>
       </c>
       <c r="F167">
@@ -3844,8 +4313,12 @@
       <c r="J167">
         <v>51.464893071194197</v>
       </c>
-    </row>
-    <row r="168" spans="1:10">
+      <c r="K167">
+        <f t="shared" si="2"/>
+        <v>64278516.359090798</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11">
       <c r="A168" s="1">
         <v>41579</v>
       </c>
@@ -3856,7 +4329,7 @@
         <v>17056.75</v>
       </c>
       <c r="E168">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.5550942406225107E-3</v>
       </c>
       <c r="F168">
@@ -3874,8 +4347,12 @@
       <c r="J168">
         <v>51.464893071194197</v>
       </c>
-    </row>
-    <row r="169" spans="1:10">
+      <c r="K168">
+        <f t="shared" si="2"/>
+        <v>64278516.359090798</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11">
       <c r="A169" s="1">
         <v>41609</v>
       </c>
@@ -3889,7 +4366,7 @@
         <v>17135</v>
       </c>
       <c r="E169">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.5872432010948643E-3</v>
       </c>
       <c r="F169">
@@ -3907,8 +4384,12 @@
       <c r="J169">
         <v>51.464893071194197</v>
       </c>
-    </row>
-    <row r="170" spans="1:10">
+      <c r="K169">
+        <f t="shared" si="2"/>
+        <v>64905405.429025702</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11">
       <c r="A170" s="1">
         <v>41640</v>
       </c>
@@ -3919,7 +4400,7 @@
         <v>17218.833333333332</v>
       </c>
       <c r="E170">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.5283639389515351E-3</v>
       </c>
       <c r="F170">
@@ -3937,8 +4418,12 @@
       <c r="J170">
         <v>51.464893071194197</v>
       </c>
-    </row>
-    <row r="171" spans="1:10">
+      <c r="K170">
+        <f t="shared" si="2"/>
+        <v>66159183.568895496</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11">
       <c r="A171" s="1">
         <v>41671</v>
       </c>
@@ -3949,7 +4434,7 @@
         <v>17302.666666666668</v>
       </c>
       <c r="E171">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.4998957357506161E-3</v>
       </c>
       <c r="F171">
@@ -3967,8 +4452,12 @@
       <c r="J171">
         <v>51.464893071194197</v>
       </c>
-    </row>
-    <row r="172" spans="1:10">
+      <c r="K171">
+        <f t="shared" si="2"/>
+        <v>66786072.638830401</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11">
       <c r="A172" s="1">
         <v>41699</v>
       </c>
@@ -3979,7 +4468,7 @@
         <v>17386.5</v>
       </c>
       <c r="E172">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.5176064608264165E-3</v>
       </c>
       <c r="F172">
@@ -3997,8 +4486,12 @@
       <c r="J172">
         <v>51.464893071194197</v>
       </c>
-    </row>
-    <row r="173" spans="1:10">
+      <c r="K172">
+        <f t="shared" si="2"/>
+        <v>66786072.638830401</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11">
       <c r="A173" s="1">
         <v>41730</v>
       </c>
@@ -4009,7 +4502,7 @@
         <v>17470.333333333332</v>
       </c>
       <c r="E173">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.4599478648108225E-3</v>
       </c>
       <c r="F173">
@@ -4027,8 +4520,12 @@
       <c r="J173">
         <v>51.464893071194197</v>
       </c>
-    </row>
-    <row r="174" spans="1:10">
+      <c r="K173">
+        <f t="shared" si="2"/>
+        <v>66786072.638830401</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11">
       <c r="A174" s="1">
         <v>41760</v>
       </c>
@@ -4039,7 +4536,7 @@
         <v>17554.166666666668</v>
       </c>
       <c r="E174">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.4216722644977638E-3</v>
       </c>
       <c r="F174">
@@ -4057,8 +4554,12 @@
       <c r="J174">
         <v>51.464893071194197</v>
       </c>
-    </row>
-    <row r="175" spans="1:10">
+      <c r="K174">
+        <f t="shared" si="2"/>
+        <v>66786072.638830401</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11">
       <c r="A175" s="1">
         <v>41791</v>
       </c>
@@ -4069,7 +4570,7 @@
         <v>17638</v>
       </c>
       <c r="E175">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.3553433651673376E-3</v>
       </c>
       <c r="F175">
@@ -4087,8 +4588,12 @@
       <c r="J175">
         <v>50.9468257350185</v>
       </c>
-    </row>
-    <row r="176" spans="1:10">
+      <c r="K175">
+        <f t="shared" si="2"/>
+        <v>66472628.103863001</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11">
       <c r="A176" s="1">
         <v>41821</v>
       </c>
@@ -4099,7 +4604,7 @@
         <v>17721.833333333332</v>
       </c>
       <c r="E176">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.3294028177444776E-3</v>
       </c>
       <c r="F176">
@@ -4116,6 +4621,10 @@
       </c>
       <c r="J176">
         <v>48.874556390315803</v>
+      </c>
+      <c r="K176">
+        <f t="shared" si="2"/>
+        <v>66159183.568895496</v>
       </c>
     </row>
     <row r="177" spans="1:11">
@@ -4129,7 +4638,7 @@
         <v>17805.666666666668</v>
       </c>
       <c r="E177">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.2355393410189639E-3</v>
       </c>
       <c r="F177">
@@ -4146,6 +4655,10 @@
       </c>
       <c r="J177">
         <v>46.0251860413495</v>
+      </c>
+      <c r="K177">
+        <f t="shared" si="2"/>
+        <v>65845739.033928096</v>
       </c>
     </row>
     <row r="178" spans="1:11">
@@ -4159,7 +4672,7 @@
         <v>17889.5</v>
       </c>
       <c r="E178">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.0809330413268397E-3</v>
       </c>
       <c r="F178">
@@ -4176,6 +4689,10 @@
       </c>
       <c r="J178">
         <v>43.693883028558901</v>
+      </c>
+      <c r="K178">
+        <f t="shared" si="2"/>
+        <v>65845739.033928096</v>
       </c>
     </row>
     <row r="179" spans="1:11">
@@ -4189,7 +4706,7 @@
         <v>17973.333333333332</v>
       </c>
       <c r="E179">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.955069722615264E-3</v>
       </c>
       <c r="F179">
@@ -4206,6 +4723,10 @@
       </c>
       <c r="J179">
         <v>42.916782024295401</v>
+      </c>
+      <c r="K179">
+        <f t="shared" ref="K179:K199" si="4">1000000*I179</f>
+        <v>65845739.033927999</v>
       </c>
     </row>
     <row r="180" spans="1:11">
@@ -4219,7 +4740,7 @@
         <v>18057.166666666668</v>
       </c>
       <c r="E180">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.8105376967917998E-3</v>
       </c>
       <c r="F180">
@@ -4236,6 +4757,10 @@
       </c>
       <c r="J180">
         <v>42.398714688119703</v>
+      </c>
+      <c r="K180">
+        <f t="shared" si="4"/>
+        <v>66159183.568895496</v>
       </c>
     </row>
     <row r="181" spans="1:11">
@@ -4252,7 +4777,7 @@
         <v>18141</v>
       </c>
       <c r="E181">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.6246227401443964E-3</v>
       </c>
       <c r="F181">
@@ -4271,7 +4796,8 @@
         <v>42.139681020031901</v>
       </c>
       <c r="K181">
-        <v>3.5550000000000002</v>
+        <f t="shared" si="4"/>
+        <v>66472628.103862904</v>
       </c>
     </row>
     <row r="182" spans="1:11">
@@ -4285,7 +4811,7 @@
         <v>18270.166666666668</v>
       </c>
       <c r="E182">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.4091925320026314E-3</v>
       </c>
       <c r="F182" s="10">
@@ -4302,6 +4828,10 @@
       </c>
       <c r="J182">
         <v>42.657748356207598</v>
+      </c>
+      <c r="K182">
+        <f t="shared" si="4"/>
+        <v>66786072.638830401</v>
       </c>
     </row>
     <row r="183" spans="1:11">
@@ -4315,7 +4845,7 @@
         <v>18399.333333333332</v>
       </c>
       <c r="E183">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.3089727899820836E-3</v>
       </c>
       <c r="F183" s="10">
@@ -4332,6 +4862,10 @@
       </c>
       <c r="J183">
         <v>42.916782024295401</v>
+      </c>
+      <c r="K183">
+        <f t="shared" si="4"/>
+        <v>66786072.638830401</v>
       </c>
     </row>
     <row r="184" spans="1:11">
@@ -4345,7 +4879,7 @@
         <v>18528.5</v>
       </c>
       <c r="E184">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.1727244331892805E-3</v>
       </c>
       <c r="F184" s="10">
@@ -4362,6 +4896,10 @@
       </c>
       <c r="J184">
         <v>42.916782024295401</v>
+      </c>
+      <c r="K184">
+        <f t="shared" si="4"/>
+        <v>66786072.638830401</v>
       </c>
     </row>
     <row r="185" spans="1:11">
@@ -4375,7 +4913,7 @@
         <v>18657.666666666668</v>
       </c>
       <c r="E185">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.1226096875252253E-3</v>
       </c>
       <c r="F185" s="10">
@@ -4392,6 +4930,10 @@
       </c>
       <c r="J185">
         <v>43.693883028558901</v>
+      </c>
+      <c r="K185">
+        <f t="shared" si="4"/>
+        <v>66786072.638830401</v>
       </c>
     </row>
     <row r="186" spans="1:11">
@@ -4405,7 +4947,7 @@
         <v>18786.833333333332</v>
       </c>
       <c r="E186">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.1830496069699451E-3</v>
       </c>
       <c r="F186" s="10">
@@ -4422,6 +4964,10 @@
       </c>
       <c r="J186">
         <v>43.434849360471098</v>
+      </c>
+      <c r="K186">
+        <f t="shared" si="4"/>
+        <v>66786072.638830401</v>
       </c>
     </row>
     <row r="187" spans="1:11">
@@ -4435,7 +4981,7 @@
         <v>18916</v>
       </c>
       <c r="E187">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.1297893302472567E-3</v>
       </c>
       <c r="F187" s="10">
@@ -4452,6 +4998,10 @@
       </c>
       <c r="J187">
         <v>42.139681020031901</v>
+      </c>
+      <c r="K187">
+        <f t="shared" si="4"/>
+        <v>66472628.103862904</v>
       </c>
     </row>
     <row r="188" spans="1:11">
@@ -4465,7 +5015,7 @@
         <v>19045.166666666668</v>
       </c>
       <c r="E188">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.0048970220203954E-3</v>
       </c>
       <c r="F188" s="10">
@@ -4482,6 +5032,10 @@
       </c>
       <c r="J188">
         <v>40.067411675329197</v>
+      </c>
+      <c r="K188">
+        <f t="shared" si="4"/>
+        <v>66159183.568895496</v>
       </c>
     </row>
     <row r="189" spans="1:11">
@@ -4495,7 +5049,7 @@
         <v>19174.333333333332</v>
       </c>
       <c r="E189">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.899141078301395E-3</v>
       </c>
       <c r="F189" s="10">
@@ -4512,6 +5066,10 @@
       </c>
       <c r="J189">
         <v>39.031277002977703</v>
+      </c>
+      <c r="K189">
+        <f t="shared" si="4"/>
+        <v>65845739.033927999</v>
       </c>
     </row>
     <row r="190" spans="1:11">
@@ -4525,7 +5083,7 @@
         <v>19303.5</v>
       </c>
       <c r="E190">
-        <f t="shared" ref="E190:E205" si="2">B190/D190</f>
+        <f t="shared" ref="E190:E205" si="5">B190/D190</f>
         <v>4.8242048357666715E-3</v>
       </c>
       <c r="F190" s="10">
@@ -4542,6 +5100,10 @@
       </c>
       <c r="J190">
         <v>37.9951423306264</v>
+      </c>
+      <c r="K190">
+        <f t="shared" si="4"/>
+        <v>65845739.033928096</v>
       </c>
     </row>
     <row r="191" spans="1:11">
@@ -4555,7 +5117,7 @@
         <v>19432.666666666668</v>
       </c>
       <c r="E191">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.7842012355180574E-3</v>
       </c>
       <c r="F191" s="10">
@@ -4572,6 +5134,10 @@
       </c>
       <c r="J191">
         <v>36.440940322099301</v>
+      </c>
+      <c r="K191">
+        <f t="shared" si="4"/>
+        <v>65845739.033927999</v>
       </c>
     </row>
     <row r="192" spans="1:11">
@@ -4585,7 +5151,7 @@
         <v>19561.833333333332</v>
       </c>
       <c r="E192">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.6363786164047112E-3</v>
       </c>
       <c r="F192" s="10">
@@ -4603,8 +5169,12 @@
       <c r="J192">
         <v>33.332536305045302</v>
       </c>
-    </row>
-    <row r="193" spans="1:10">
+      <c r="K192">
+        <f t="shared" si="4"/>
+        <v>65845739.033927999</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11">
       <c r="A193" s="1">
         <v>42339</v>
       </c>
@@ -4618,7 +5188,7 @@
         <v>19691</v>
       </c>
       <c r="E193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.5654977252789376E-3</v>
       </c>
       <c r="F193" s="10">
@@ -4636,8 +5206,12 @@
       <c r="J193">
         <v>30.742199624166801</v>
       </c>
-    </row>
-    <row r="194" spans="1:10">
+      <c r="K193">
+        <f t="shared" si="4"/>
+        <v>65845739.033927999</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11">
       <c r="A194" s="1">
         <v>42370</v>
       </c>
@@ -4648,7 +5222,7 @@
         <v>19711.333333333332</v>
       </c>
       <c r="E194">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.4679710024772513E-3</v>
       </c>
       <c r="F194" s="10">
@@ -4666,8 +5240,12 @@
       <c r="J194">
         <v>29.187997615639802</v>
       </c>
-    </row>
-    <row r="195" spans="1:10">
+      <c r="K194">
+        <f t="shared" si="4"/>
+        <v>65532294.498960599</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11">
       <c r="A195" s="1">
         <v>42401</v>
       </c>
@@ -4679,7 +5257,7 @@
         <v>19731.666666666668</v>
       </c>
       <c r="E195">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.4914744229248866E-3</v>
       </c>
       <c r="F195" s="10">
@@ -4697,8 +5275,12 @@
       <c r="J195">
         <v>28.669930279464101</v>
       </c>
-    </row>
-    <row r="196" spans="1:10">
+      <c r="K195">
+        <f t="shared" si="4"/>
+        <v>64591960.894058205</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11">
       <c r="A196" s="1">
         <v>42430</v>
       </c>
@@ -4710,7 +5292,7 @@
         <v>19752</v>
       </c>
       <c r="E196">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.5173318169090954E-3</v>
       </c>
       <c r="F196" s="10">
@@ -4728,8 +5310,12 @@
       <c r="J196">
         <v>28.1518629432884</v>
       </c>
-    </row>
-    <row r="197" spans="1:10">
+      <c r="K196">
+        <f t="shared" si="4"/>
+        <v>64278516.359090798</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11">
       <c r="A197" s="1">
         <v>42461</v>
       </c>
@@ -4741,7 +5327,7 @@
         <v>19772.333333333332</v>
       </c>
       <c r="E197">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.5847752999378004E-3</v>
       </c>
       <c r="F197" s="10">
@@ -4759,8 +5345,12 @@
       <c r="J197">
         <v>27.892829275200501</v>
       </c>
-    </row>
-    <row r="198" spans="1:10">
+      <c r="K197">
+        <f t="shared" si="4"/>
+        <v>63024738.219220899</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11">
       <c r="A198" s="1">
         <v>42491</v>
       </c>
@@ -4772,7 +5362,7 @@
         <v>19792.666666666668</v>
       </c>
       <c r="E198">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.5845852981924746E-3</v>
       </c>
       <c r="F198" s="10">
@@ -4787,8 +5377,12 @@
       <c r="I198">
         <v>62.711293684253398</v>
       </c>
-    </row>
-    <row r="199" spans="1:10">
+      <c r="K198">
+        <f t="shared" si="4"/>
+        <v>62711293.684253402</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11">
       <c r="A199" s="1">
         <v>42522</v>
       </c>
@@ -4800,7 +5394,7 @@
         <v>19813</v>
       </c>
       <c r="E199">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.6102314936741079E-3</v>
       </c>
       <c r="F199" s="10">
@@ -4815,8 +5409,12 @@
       <c r="I199">
         <v>62.084404614318501</v>
       </c>
-    </row>
-    <row r="200" spans="1:10">
+      <c r="K199">
+        <f t="shared" si="4"/>
+        <v>62084404.614318497</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11">
       <c r="A200" s="1">
         <v>42552</v>
       </c>
@@ -4828,7 +5426,7 @@
         <v>19833.333333333332</v>
       </c>
       <c r="E200">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.5858380950147921E-3</v>
       </c>
       <c r="F200" s="10">
@@ -4841,7 +5439,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:11">
       <c r="A201" s="1">
         <v>42583</v>
       </c>
@@ -4853,7 +5451,7 @@
         <v>19853.666666666668</v>
       </c>
       <c r="E201">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.6194722567574238E-3</v>
       </c>
       <c r="F201" s="10">
@@ -4866,7 +5464,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:11">
       <c r="A202" s="1">
         <v>42614</v>
       </c>
@@ -4878,7 +5476,7 @@
         <v>19874</v>
       </c>
       <c r="E202">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.6175873768676155E-3</v>
       </c>
       <c r="F202" s="10">
@@ -4891,7 +5489,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:11">
       <c r="A203" s="1">
         <v>42644</v>
       </c>
@@ -4903,7 +5501,7 @@
         <v>19894.333333333332</v>
       </c>
       <c r="E203">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.6233540679451977E-3</v>
       </c>
       <c r="F203" s="10">
@@ -4916,7 +5514,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:11">
       <c r="A204" s="1">
         <v>42675</v>
       </c>
@@ -4928,7 +5526,7 @@
         <v>19914.666666666668</v>
       </c>
       <c r="E204">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.5816260554969552E-3</v>
       </c>
       <c r="F204" s="10">
@@ -4941,7 +5539,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:11">
       <c r="A205" s="1">
         <v>42705</v>
       </c>
@@ -4955,7 +5553,7 @@
         <v>19935</v>
       </c>
       <c r="E205">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.5965811303030103E-3</v>
       </c>
       <c r="F205" s="10">
@@ -4968,7 +5566,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:11">
       <c r="A206" t="s">
         <v>36</v>
       </c>
@@ -4994,11 +5592,11 @@
         <v>57.161043432445858</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:11">
       <c r="B207" s="2"/>
       <c r="F207" s="10"/>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:11">
       <c r="B208" s="2"/>
       <c r="F208" s="10"/>
     </row>
@@ -5924,6 +6522,233 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E17147-9981-8A4C-9D06-BC7C6FB55E00}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21" thickBot="1"/>
+    <row r="3" spans="1:9">
+      <c r="A3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="8"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.79817814978501889</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.63708835879423598</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.63443936871244211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="5">
+        <v>10092928.995099191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="21" thickBot="1">
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="6">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="21" thickBot="1">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5">
+        <v>2.4499305494331932E+16</v>
+      </c>
+      <c r="D12" s="5">
+        <v>2.4499305494331932E+16</v>
+      </c>
+      <c r="E12" s="5">
+        <v>240.50235717107682</v>
+      </c>
+      <c r="F12" s="5">
+        <v>5.9605568569202832E-32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="5">
+        <v>137</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1.3955808550915612E+16</v>
+      </c>
+      <c r="D13" s="5">
+        <v>101867215700113.95</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" ht="21" thickBot="1">
+      <c r="A14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="6">
+        <v>138</v>
+      </c>
+      <c r="C14" s="6">
+        <v>3.8455114045247544E+16</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" ht="21" thickBot="1"/>
+    <row r="16" spans="1:9">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="5">
+        <v>17854157.170421883</v>
+      </c>
+      <c r="C17" s="5">
+        <v>4025824.2588552344</v>
+      </c>
+      <c r="D17" s="5">
+        <v>4.4349072444356556</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1.8748051823539615E-5</v>
+      </c>
+      <c r="F17" s="5">
+        <v>9893366.6256941184</v>
+      </c>
+      <c r="G17" s="5">
+        <v>25814947.715149648</v>
+      </c>
+      <c r="H17" s="5">
+        <v>9893366.6256941184</v>
+      </c>
+      <c r="I17" s="5">
+        <v>25814947.715149648</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="21" thickBot="1">
+      <c r="A18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="6">
+        <v>7944484914.483717</v>
+      </c>
+      <c r="C18" s="6">
+        <v>512278437.34008533</v>
+      </c>
+      <c r="D18" s="6">
+        <v>15.508138417330313</v>
+      </c>
+      <c r="E18" s="6">
+        <v>5.960556856920708E-32</v>
+      </c>
+      <c r="F18" s="6">
+        <v>6931489543.0949745</v>
+      </c>
+      <c r="G18" s="6">
+        <v>8957480285.8724594</v>
+      </c>
+      <c r="H18" s="6">
+        <v>6931489543.0949745</v>
+      </c>
+      <c r="I18" s="6">
+        <v>8957480285.8724594</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778AA02C-85B6-8441-AC36-F432356D488B}">
   <dimension ref="A1:I18"/>
   <sheetViews>

</xml_diff>